<commit_message>
ganesh - Committing with gApps.java file
</commit_message>
<xml_diff>
--- a/CRAFT_mCRAFT/Datatables/MobileTestingScenario.xlsx
+++ b/CRAFT_mCRAFT/Datatables/MobileTestingScenario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14205" windowHeight="4665" tabRatio="721"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13830" windowHeight="3255" tabRatio="721"/>
   </bookViews>
   <sheets>
     <sheet name="Business_Flow" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Parametrized_Checkpoints" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -831,7 +832,7 @@
     <t>runLoopTest</t>
   </si>
   <si>
-    <t>ScenarioExecution1</t>
+    <t>gTest</t>
   </si>
 </sst>
 </file>
@@ -1215,13 +1216,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV8"/>
+  <dimension ref="A1:IV9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2060,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:256" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>271</v>
       </c>
@@ -2067,6 +2068,7 @@
         <v>271</v>
       </c>
     </row>
+    <row r="9" spans="1:256" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>